<commit_message>
Removed the emoji in the cleaned up text
</commit_message>
<xml_diff>
--- a/ads_mini_project/scrapedata/12083.xlsx
+++ b/ads_mini_project/scrapedata/12083.xlsx
@@ -1159,7 +1159,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>welcome 😊</t>
+          <t>welcome</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>welcome 😊</t>
+          <t>welcome</t>
         </is>
       </c>
     </row>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>welcome 😊</t>
+          <t>welcome</t>
         </is>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>it’s annoy thing samsung remove feature face s22 ultra really annoy use feature lot</t>
+          <t>annoy thing samsung remove feature face s22 ultra really annoy use feature lot</t>
         </is>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>third know issue 😇</t>
+          <t>third know issue</t>
         </is>
       </c>
     </row>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>wed get sseries phone 6364 inch display 😏</t>
+          <t>wed get sseries phone 6364 inch display</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>it’s annoy thing samsung remove feature face s22 ultra really annoy use feature lot</t>
+          <t>annoy thing samsung remove feature face s22 ultra really annoy use feature lot</t>
         </is>
       </c>
     </row>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>third know issue 😇</t>
+          <t>third know issue</t>
         </is>
       </c>
     </row>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>wed get sseries phone 6364 inch display 😏</t>
+          <t>wed get sseries phone 6364 inch display</t>
         </is>
       </c>
     </row>
@@ -4627,7 +4627,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>today buy third s23 row banana blur main camera yes take photos document nicely 3x zoom refuse €1000 phone old 4 year phone dont even want see phone anymore sm916bdb make vietnam 512gb version</t>
+          <t>today buy third s23 row banana blur main camera yes take photos document nicely 3x zoom refuse 1000 phone old 4 year phone dont even want see phone anymore sm916bdb make vietnam 512gb version</t>
         </is>
       </c>
     </row>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>it’s annoy thing samsung remove feature face s22 ultra really annoy use feature lot</t>
+          <t>annoy thing samsung remove feature face s22 ultra really annoy use feature lot</t>
         </is>
       </c>
     </row>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>third know issue 😇</t>
+          <t>third know issue</t>
         </is>
       </c>
     </row>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>wed get sseries phone 6364 inch display 😏</t>
+          <t>wed get sseries phone 6364 inch display</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>today buy third s23 row banana blur main camera yes take photos document nicely 3x zoom refuse €1000 phone old 4 year phone dont even want see phone anymore sm916bdb make vietnam 512gb version</t>
+          <t>today buy third s23 row banana blur main camera yes take photos document nicely 3x zoom refuse 1000 phone old 4 year phone dont even want see phone anymore sm916bdb make vietnam 512gb version</t>
         </is>
       </c>
     </row>
@@ -6450,7 +6450,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>today buy third s23 row banana blur main camera yes take photos document nicely 3x zoom refuse €1000 phone old 4 year phone dont even want see phone anymore sm916bdb make vietnam 512gb version</t>
+          <t>today buy third s23 row banana blur main camera yes take photos document nicely 3x zoom refuse 1000 phone old 4 year phone dont even want see phone anymore sm916bdb make vietnam 512gb version</t>
         </is>
       </c>
     </row>
@@ -7428,7 +7428,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>it’s middle get base s23 feature small size either advantage disadvantage small battery get s23 ultra spend get feature like spen 2k screen 10x telephoto etc</t>
+          <t>middle get base s23 feature small size either advantage disadvantage small battery get s23 ultra spend get feature like spen 2k screen 10x telephoto etc</t>
         </is>
       </c>
     </row>
@@ -8346,7 +8346,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>it’s middle get base s23 feature small size either advantage disadvantage small battery get s23 ultra spend get feature like spen 2k screen 10x telephoto etc</t>
+          <t>middle get base s23 feature small size either advantage disadvantage small battery get s23 ultra spend get feature like spen 2k screen 10x telephoto etc</t>
         </is>
       </c>
     </row>
@@ -8953,7 +8953,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>well say 👍🏻</t>
+          <t>well say</t>
         </is>
       </c>
     </row>
@@ -9264,7 +9264,7 @@
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>it’s middle get base s23 feature small size either advantage disadvantage small battery get s23 ultra spend get feature like spen 2k screen 10x telephoto etc</t>
+          <t>middle get base s23 feature small size either advantage disadvantage small battery get s23 ultra spend get feature like spen 2k screen 10x telephoto etc</t>
         </is>
       </c>
     </row>
@@ -9871,7 +9871,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>well say 👍🏻</t>
+          <t>well say</t>
         </is>
       </c>
     </row>
@@ -10185,7 +10185,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>yes exynos 2400 confirm s24 plus india europe s24 plus sms926b spot geekbench exynos 2400 processor 8gb ram • single 2067 similar less 8gen2 • multi 6520</t>
+          <t>yes exynos 2400 confirm s24 plus india europe s24 plus sms926b spot geekbench exynos 2400 processor 8gb ram single 2067 similar less 8gen2 multi 6520</t>
         </is>
       </c>
     </row>
@@ -10767,7 +10767,7 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>well say 👍🏻</t>
+          <t>well say</t>
         </is>
       </c>
     </row>
@@ -11081,7 +11081,7 @@
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>yes exynos 2400 confirm s24 plus india europe s24 plus sms926b spot geekbench exynos 2400 processor 8gb ram • single 2067 similar less 8gen2 • multi 6520</t>
+          <t>yes exynos 2400 confirm s24 plus india europe s24 plus sms926b spot geekbench exynos 2400 processor 8gb ram single 2067 similar less 8gen2 multi 6520</t>
         </is>
       </c>
     </row>
@@ -11965,7 +11965,7 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>yes exynos 2400 confirm s24 plus india europe s24 plus sms926b spot geekbench exynos 2400 processor 8gb ram • single 2067 similar less 8gen2 • multi 6520</t>
+          <t>yes exynos 2400 confirm s24 plus india europe s24 plus sms926b spot geekbench exynos 2400 processor 8gb ram single 2067 similar less 8gen2 multi 6520</t>
         </is>
       </c>
     </row>
@@ -12808,7 +12808,7 @@
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>buy £699 tradein break phone get free silicone case 12 month disney £10 store voucher plus stuff samsung boost make essentially £600 phone half price iphonepm flagship experience nice one samsung</t>
+          <t>buy 699 tradein broken phone get free silicone case 12 month disney 10 store voucher plus stuff samsung boost make essentially 600 phone half price iphonepm flagship experience nice one samsung</t>
         </is>
       </c>
     </row>
@@ -13053,7 +13053,7 @@
       </c>
       <c r="D559" t="inlineStr">
         <is>
-          <t>well time samsung improve battery capacity line 4700mah 2023 ®©</t>
+          <t>well time samsung improve battery capacity line 4700mah 2023</t>
         </is>
       </c>
     </row>
@@ -13696,7 +13696,7 @@
       </c>
       <c r="D588" t="inlineStr">
         <is>
-          <t>buy £699 tradein break phone get free silicone case 12 month disney £10 store voucher plus stuff samsung boost make essentially £600 phone half price iphonepm flagship experience nice one samsung</t>
+          <t>buy 699 tradein broken phone get free silicone case 12 month disney 10 store voucher plus stuff samsung boost make essentially 600 phone half price iphonepm flagship experience nice one samsung</t>
         </is>
       </c>
     </row>
@@ -13941,7 +13941,7 @@
       </c>
       <c r="D599" t="inlineStr">
         <is>
-          <t>well time samsung improve battery capacity line 4700mah 2023 ®©</t>
+          <t>well time samsung improve battery capacity line 4700mah 2023</t>
         </is>
       </c>
     </row>
@@ -14051,7 +14051,7 @@
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>s20 sereies fine camera form s21 issue exist non pro sereies may s24 launch superb camera samsung change camera module s24 plus👍</t>
+          <t>s20 sereies fine camera form s21 issue exist non pro sereies may s24 launch superb camera samsung change camera module s24 plus</t>
         </is>
       </c>
     </row>
@@ -14589,7 +14589,7 @@
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>buy £699 tradein break phone get free silicone case 12 month disney £10 store voucher plus stuff samsung boost make essentially £600 phone half price iphonepm flagship experience nice one samsung</t>
+          <t>buy 699 tradein broken phone get free silicone case 12 month disney 10 store voucher plus stuff samsung boost make essentially 600 phone half price iphonepm flagship experience nice one samsung</t>
         </is>
       </c>
     </row>
@@ -14834,7 +14834,7 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>well time samsung improve battery capacity line 4700mah 2023 ®©</t>
+          <t>well time samsung improve battery capacity line 4700mah 2023</t>
         </is>
       </c>
     </row>
@@ -14944,7 +14944,7 @@
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>s20 sereies fine camera form s21 issue exist non pro sereies may s24 launch superb camera samsung change camera module s24 plus👍</t>
+          <t>s20 sereies fine camera form s21 issue exist non pro sereies may s24 launch superb camera samsung change camera module s24 plus</t>
         </is>
       </c>
     </row>
@@ -15525,7 +15525,7 @@
       </c>
       <c r="D670" t="inlineStr">
         <is>
-          <t>samsung upgrade display s24 sereies wqhd instead fhd 65 watt charge new camera lens setup blur issue perfect phone👍</t>
+          <t>samsung upgrade display s24 sereies wqhd instead fhd 65 watt charge new camera lens setup blur issue perfect phone</t>
         </is>
       </c>
     </row>
@@ -15683,7 +15683,7 @@
       </c>
       <c r="D677" t="inlineStr">
         <is>
-          <t>confirm get s23 plus today absolutely blurry banana 🍌 issue handset even try close issue photo wonderfully crisp</t>
+          <t>confirm get s23 plus today absolutely blurry banana issue handset even try close issue photo wonderfully crisp</t>
         </is>
       </c>
     </row>
@@ -15750,7 +15750,7 @@
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>software remove compensate lens aberration sad 5 year revert purchased samsung galaxy s23 use brand 😖</t>
+          <t>software remove compensate lens aberration sad 5 year revert purchased samsung galaxy s23 use brand</t>
         </is>
       </c>
     </row>
@@ -15838,7 +15838,7 @@
       </c>
       <c r="D684" t="inlineStr">
         <is>
-          <t>s20 sereies fine camera form s21 issue exist non pro sereies may s24 launch superb camera samsung change camera module s24 plus👍</t>
+          <t>s20 sereies fine camera form s21 issue exist non pro sereies may s24 launch superb camera samsung change camera module s24 plus</t>
         </is>
       </c>
     </row>
@@ -16419,7 +16419,7 @@
       </c>
       <c r="D710" t="inlineStr">
         <is>
-          <t>samsung upgrade display s24 sereies wqhd instead fhd 65 watt charge new camera lens setup blur issue perfect phone👍</t>
+          <t>samsung upgrade display s24 sereies wqhd instead fhd 65 watt charge new camera lens setup blur issue perfect phone</t>
         </is>
       </c>
     </row>
@@ -16577,7 +16577,7 @@
       </c>
       <c r="D717" t="inlineStr">
         <is>
-          <t>confirm get s23 plus today absolutely blurry banana 🍌 issue handset even try close issue photo wonderfully crisp</t>
+          <t>confirm get s23 plus today absolutely blurry banana issue handset even try close issue photo wonderfully crisp</t>
         </is>
       </c>
     </row>
@@ -16644,7 +16644,7 @@
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>software remove compensate lens aberration sad 5 year revert purchased samsung galaxy s23 use brand 😖</t>
+          <t>software remove compensate lens aberration sad 5 year revert purchased samsung galaxy s23 use brand</t>
         </is>
       </c>
     </row>
@@ -17020,7 +17020,7 @@
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>im disappoint samsung s23 plus bad camera market every photo get blurry circle shape cant make good quality photo flagdownship samsung samsung support team shameless liar samsung tell camera feature feature feature poor quality photo real huge issue In My Honest/Humble Opinion lens problem software almost photo take samsung s23 camera low quality worthless flagship please think buy please google s23 bananagete problem 😔 thank wish happiness 😊</t>
+          <t>im disappoint samsung s23 plus bad camera market every photo get blurry circle shape cant make good quality photo flagdownship samsung samsung support team shameless liar samsung tell camera feature feature feature poor quality photo real huge issue In My HonestHumble Opinion lens problem software almost photo take samsung s23 camera low quality worthless flagship please think buy please google s23 bananagete problem thank wish happiness</t>
         </is>
       </c>
     </row>
@@ -17064,7 +17064,7 @@
       </c>
       <c r="D739" t="inlineStr">
         <is>
-          <t>oxygenos bad os oneui saw somewhere discord oxygenos really responsive bit confused 😅</t>
+          <t>oxygenos bad os oneui saw somewhere discord oxygenos really responsive bit confuse</t>
         </is>
       </c>
     </row>
@@ -17323,7 +17323,7 @@
       </c>
       <c r="D750" t="inlineStr">
         <is>
-          <t>samsung upgrade display s24 sereies wqhd instead fhd 65 watt charge new camera lens setup blur issue perfect phone👍</t>
+          <t>samsung upgrade display s24 sereies wqhd instead fhd 65 watt charge new camera lens setup blur issue perfect phone</t>
         </is>
       </c>
     </row>
@@ -17481,7 +17481,7 @@
       </c>
       <c r="D757" t="inlineStr">
         <is>
-          <t>confirm get s23 plus today absolutely blurry banana 🍌 issue handset even try close issue photo wonderfully crisp</t>
+          <t>confirm get s23 plus today absolutely blurry banana issue handset even try close issue photo wonderfully crisp</t>
         </is>
       </c>
     </row>
@@ -17548,7 +17548,7 @@
       </c>
       <c r="D760" t="inlineStr">
         <is>
-          <t>software remove compensate lens aberration sad 5 year revert purchased samsung galaxy s23 use brand 😖</t>
+          <t>software remove compensate lens aberration sad 5 year revert purchased samsung galaxy s23 use brand</t>
         </is>
       </c>
     </row>
@@ -17924,7 +17924,7 @@
       </c>
       <c r="D777" t="inlineStr">
         <is>
-          <t>im disappoint samsung s23 plus bad camera market every photo get blurry circle shape cant make good quality photo flagdownship samsung samsung support team shameless liar samsung tell camera feature feature feature poor quality photo real huge issue In My Honest/Humble Opinion lens problem software almost photo take samsung s23 camera low quality worthless flagship please think buy please google s23 bananagete problem 😔 thank wish happiness 😊</t>
+          <t>im disappoint samsung s23 plus bad camera market every photo get blurry circle shape cant make good quality photo flagdownship samsung samsung support team shameless liar samsung tell camera feature feature feature poor quality photo real huge issue In My HonestHumble Opinion lens problem software almost photo take samsung s23 camera low quality worthless flagship please think buy please google s23 bananagete problem thank wish happiness</t>
         </is>
       </c>
     </row>
@@ -17968,7 +17968,7 @@
       </c>
       <c r="D779" t="inlineStr">
         <is>
-          <t>oxygenos bad os oneui saw somewhere discord oxygenos really responsive bit confused 😅</t>
+          <t>oxygenos bad os oneui saw somewhere discord oxygenos really responsive bit confuse</t>
         </is>
       </c>
     </row>
@@ -18088,7 +18088,7 @@
       </c>
       <c r="D784" t="inlineStr">
         <is>
-          <t>june 22gb big update available india today 🇮🇳</t>
+          <t>june 22gb big update available india today</t>
         </is>
       </c>
     </row>
@@ -18204,7 +18204,7 @@
       </c>
       <c r="D789" t="inlineStr">
         <is>
-          <t>case mine today s23 show check chargerusb port moisture detect chargerusb port make sure dry charge phone humid weather 🤔</t>
+          <t>case mine today s23 show check chargerusb port moisture detect chargerusb port make sure dry charge phone humid weather</t>
         </is>
       </c>
     </row>
@@ -18348,7 +18348,7 @@
       </c>
       <c r="D795" t="inlineStr">
         <is>
-          <t>nice 👏🏼</t>
+          <t>nice</t>
         </is>
       </c>
     </row>
@@ -18836,7 +18836,7 @@
       </c>
       <c r="D817" t="inlineStr">
         <is>
-          <t>im disappoint samsung s23 plus bad camera market every photo get blurry circle shape cant make good quality photo flagdownship samsung samsung support team shameless liar samsung tell camera feature feature feature poor quality photo real huge issue In My Honest/Humble Opinion lens problem software almost photo take samsung s23 camera low quality worthless flagship please think buy please google s23 bananagete problem 😔 thank wish happiness 😊</t>
+          <t>im disappoint samsung s23 plus bad camera market every photo get blurry circle shape cant make good quality photo flagdownship samsung samsung support team shameless liar samsung tell camera feature feature feature poor quality photo real huge issue In My HonestHumble Opinion lens problem software almost photo take samsung s23 camera low quality worthless flagship please think buy please google s23 bananagete problem thank wish happiness</t>
         </is>
       </c>
     </row>
@@ -18880,7 +18880,7 @@
       </c>
       <c r="D819" t="inlineStr">
         <is>
-          <t>oxygenos bad os oneui saw somewhere discord oxygenos really responsive bit confused 😅</t>
+          <t>oxygenos bad os oneui saw somewhere discord oxygenos really responsive bit confuse</t>
         </is>
       </c>
     </row>
@@ -19000,7 +19000,7 @@
       </c>
       <c r="D824" t="inlineStr">
         <is>
-          <t>june 22gb big update available india today 🇮🇳</t>
+          <t>june 22gb big update available india today</t>
         </is>
       </c>
     </row>
@@ -19116,7 +19116,7 @@
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>case mine today s23 show check chargerusb port moisture detect chargerusb port make sure dry charge phone humid weather 🤔</t>
+          <t>case mine today s23 show check chargerusb port moisture detect chargerusb port make sure dry charge phone humid weather</t>
         </is>
       </c>
     </row>
@@ -19260,7 +19260,7 @@
       </c>
       <c r="D835" t="inlineStr">
         <is>
-          <t>nice 👏🏼</t>
+          <t>nice</t>
         </is>
       </c>
     </row>
@@ -19844,7 +19844,7 @@
       </c>
       <c r="D861" t="inlineStr">
         <is>
-          <t>s23 doesnt fm radio youre recommend a34 great joke man 😂</t>
+          <t>s23 doesnt fm radio youre recommend a34 great joke man</t>
         </is>
       </c>
     </row>
@@ -19891,7 +19891,7 @@
       </c>
       <c r="D863" t="inlineStr">
         <is>
-          <t>new rumor claim samsung may fail solve galaxy s23 camera issue it’s work past week company may supposedly delay june update whether postpone release july unclear wonder s23 weak saleslol hopefully solve s23 camera problem even possible launch s24</t>
+          <t>new rumor claim samsung may fail solve galaxy s23 camera issue work past week company may supposedly delay june update whether postpone release july unclear wonder s23 weak saleslol hopefully solve s23 camera problem even possible launch s24</t>
         </is>
       </c>
     </row>
@@ -19913,7 +19913,7 @@
       </c>
       <c r="D864" t="inlineStr">
         <is>
-          <t>june 22gb big update available india today 🇮🇳</t>
+          <t>june 22gb big update available india today</t>
         </is>
       </c>
     </row>
@@ -20029,7 +20029,7 @@
       </c>
       <c r="D869" t="inlineStr">
         <is>
-          <t>case mine today s23 show check chargerusb port moisture detect chargerusb port make sure dry charge phone humid weather 🤔</t>
+          <t>case mine today s23 show check chargerusb port moisture detect chargerusb port make sure dry charge phone humid weather</t>
         </is>
       </c>
     </row>
@@ -20173,7 +20173,7 @@
       </c>
       <c r="D875" t="inlineStr">
         <is>
-          <t>nice 👏🏼</t>
+          <t>nice</t>
         </is>
       </c>
     </row>
@@ -20757,7 +20757,7 @@
       </c>
       <c r="D901" t="inlineStr">
         <is>
-          <t>s23 doesnt fm radio youre recommend a34 great joke man 😂</t>
+          <t>s23 doesnt fm radio youre recommend a34 great joke man</t>
         </is>
       </c>
     </row>
@@ -20804,7 +20804,7 @@
       </c>
       <c r="D903" t="inlineStr">
         <is>
-          <t>new rumor claim samsung may fail solve galaxy s23 camera issue it’s work past week company may supposedly delay june update whether postpone release july unclear wonder s23 weak saleslol hopefully solve s23 camera problem even possible launch s24</t>
+          <t>new rumor claim samsung may fail solve galaxy s23 camera issue work past week company may supposedly delay june update whether postpone release july unclear wonder s23 weak saleslol hopefully solve s23 camera problem even possible launch s24</t>
         </is>
       </c>
     </row>
@@ -21079,7 +21079,7 @@
       </c>
       <c r="D915" t="inlineStr">
         <is>
-          <t>people complain shutter sound another way mute 🔇 shutter sound disturb turn simple shoot without sound</t>
+          <t>people complain shutter sound another way mute shutter sound disturb turn simple shoot without sound</t>
         </is>
       </c>
     </row>
@@ -21665,7 +21665,7 @@
       </c>
       <c r="D941" t="inlineStr">
         <is>
-          <t>s23 doesnt fm radio youre recommend a34 great joke man 😂</t>
+          <t>s23 doesnt fm radio youre recommend a34 great joke man</t>
         </is>
       </c>
     </row>
@@ -21712,7 +21712,7 @@
       </c>
       <c r="D943" t="inlineStr">
         <is>
-          <t>new rumor claim samsung may fail solve galaxy s23 camera issue it’s work past week company may supposedly delay june update whether postpone release july unclear wonder s23 weak saleslol hopefully solve s23 camera problem even possible launch s24</t>
+          <t>new rumor claim samsung may fail solve galaxy s23 camera issue work past week company may supposedly delay june update whether postpone release july unclear wonder s23 weak saleslol hopefully solve s23 camera problem even possible launch s24</t>
         </is>
       </c>
     </row>
@@ -21987,7 +21987,7 @@
       </c>
       <c r="D955" t="inlineStr">
         <is>
-          <t>people complain shutter sound another way mute 🔇 shutter sound disturb turn simple shoot without sound</t>
+          <t>people complain shutter sound another way mute shutter sound disturb turn simple shoot without sound</t>
         </is>
       </c>
     </row>
@@ -22189,7 +22189,7 @@
       </c>
       <c r="D964" t="inlineStr">
         <is>
-          <t>cannot find shutter sound option anywhere s21 fe watch lot video youtube regard could find turn system sound switch silent mode 😢</t>
+          <t>cannot find shutter sound option anywhere s21 fe watch lot video youtube regard could find turn system sound switch silent mode</t>
         </is>
       </c>
     </row>
@@ -22370,7 +22370,7 @@
       </c>
       <c r="D971" t="inlineStr">
         <is>
-          <t>qualcomm snapdragon 8 gen 2 tsmc n4 1 x arm cortexx3 – 345 ghz 2 x arm cortexa715 – 30 ghz 2 x arm cortexa710 – 28 ghz 4 x arm cortexa510 – 20 ghz july 2023 qualcomm snapdragon 8 gen 3 tsmc n4 1 x arm cortexx4 – 37 ghz 2 x arm cortexa716 – 32 ghz 2 x arm cortexa711 – 30 ghz 4 x arm cortexa510 – 20 ghz november 2023</t>
+          <t>qualcomm snapdragon 8 gen 2 tsmc n4 1 x arm cortexx3 345 ghz 2 x arm cortexa715 30 ghz 2 x arm cortexa710 28 ghz 4 x arm cortexa510 20 ghz july 2023 qualcomm snapdragon 8 gen 3 tsmc n4 1 x arm cortexx4 37 ghz 2 x arm cortexa716 32 ghz 2 x arm cortexa711 30 ghz 4 x arm cortexa510 20 ghz november 2023</t>
         </is>
       </c>
     </row>
@@ -22591,7 +22591,7 @@
       </c>
       <c r="D981" t="inlineStr">
         <is>
-          <t>yes ive experienced s21 ultra quite bulky need tighten trouser bite put pocket 😳</t>
+          <t>yes ive experienced s21 ultra quite bulky need tighten trouser bite put pocket</t>
         </is>
       </c>
     </row>
@@ -22912,7 +22912,7 @@
       </c>
       <c r="D995" t="inlineStr">
         <is>
-          <t>people complain shutter sound another way mute 🔇 shutter sound disturb turn simple shoot without sound</t>
+          <t>people complain shutter sound another way mute shutter sound disturb turn simple shoot without sound</t>
         </is>
       </c>
     </row>
@@ -23114,7 +23114,7 @@
       </c>
       <c r="D1004" t="inlineStr">
         <is>
-          <t>cannot find shutter sound option anywhere s21 fe watch lot video youtube regard could find turn system sound switch silent mode 😢</t>
+          <t>cannot find shutter sound option anywhere s21 fe watch lot video youtube regard could find turn system sound switch silent mode</t>
         </is>
       </c>
     </row>
@@ -23295,7 +23295,7 @@
       </c>
       <c r="D1011" t="inlineStr">
         <is>
-          <t>qualcomm snapdragon 8 gen 2 tsmc n4 1 x arm cortexx3 – 345 ghz 2 x arm cortexa715 – 30 ghz 2 x arm cortexa710 – 28 ghz 4 x arm cortexa510 – 20 ghz july 2023 qualcomm snapdragon 8 gen 3 tsmc n4 1 x arm cortexx4 – 37 ghz 2 x arm cortexa716 – 32 ghz 2 x arm cortexa711 – 30 ghz 4 x arm cortexa510 – 20 ghz november 2023</t>
+          <t>qualcomm snapdragon 8 gen 2 tsmc n4 1 x arm cortexx3 345 ghz 2 x arm cortexa715 30 ghz 2 x arm cortexa710 28 ghz 4 x arm cortexa510 20 ghz july 2023 qualcomm snapdragon 8 gen 3 tsmc n4 1 x arm cortexx4 37 ghz 2 x arm cortexa716 32 ghz 2 x arm cortexa711 30 ghz 4 x arm cortexa510 20 ghz november 2023</t>
         </is>
       </c>
     </row>
@@ -23516,7 +23516,7 @@
       </c>
       <c r="D1021" t="inlineStr">
         <is>
-          <t>yes ive experienced s21 ultra quite bulky need tighten trouser bite put pocket 😳</t>
+          <t>yes ive experienced s21 ultra quite bulky need tighten trouser bite put pocket</t>
         </is>
       </c>
     </row>
@@ -23983,7 +23983,7 @@
       </c>
       <c r="D1042" t="inlineStr">
         <is>
-          <t>s23 plus top quality display vivid sharp bright color look natural ✨️ problem watherever fhd qhd 4k 8k pleasure watch movee</t>
+          <t>s23 plus top quality display vivid sharp bright color look natural problem watherever fhd qhd 4k 8k pleasure watch movee</t>
         </is>
       </c>
     </row>
@@ -24030,7 +24030,7 @@
       </c>
       <c r="D1044" t="inlineStr">
         <is>
-          <t>cannot find shutter sound option anywhere s21 fe watch lot video youtube regard could find turn system sound switch silent mode 😢</t>
+          <t>cannot find shutter sound option anywhere s21 fe watch lot video youtube regard could find turn system sound switch silent mode</t>
         </is>
       </c>
     </row>
@@ -24211,7 +24211,7 @@
       </c>
       <c r="D1051" t="inlineStr">
         <is>
-          <t>qualcomm snapdragon 8 gen 2 tsmc n4 1 x arm cortexx3 – 345 ghz 2 x arm cortexa715 – 30 ghz 2 x arm cortexa710 – 28 ghz 4 x arm cortexa510 – 20 ghz july 2023 qualcomm snapdragon 8 gen 3 tsmc n4 1 x arm cortexx4 – 37 ghz 2 x arm cortexa716 – 32 ghz 2 x arm cortexa711 – 30 ghz 4 x arm cortexa510 – 20 ghz november 2023</t>
+          <t>qualcomm snapdragon 8 gen 2 tsmc n4 1 x arm cortexx3 345 ghz 2 x arm cortexa715 30 ghz 2 x arm cortexa710 28 ghz 4 x arm cortexa510 20 ghz july 2023 qualcomm snapdragon 8 gen 3 tsmc n4 1 x arm cortexx4 37 ghz 2 x arm cortexa716 32 ghz 2 x arm cortexa711 30 ghz 4 x arm cortexa510 20 ghz november 2023</t>
         </is>
       </c>
     </row>
@@ -24432,7 +24432,7 @@
       </c>
       <c r="D1061" t="inlineStr">
         <is>
-          <t>yes ive experienced s21 ultra quite bulky need tighten trouser bite put pocket 😳</t>
+          <t>yes ive experienced s21 ultra quite bulky need tighten trouser bite put pocket</t>
         </is>
       </c>
     </row>
@@ -24899,7 +24899,7 @@
       </c>
       <c r="D1082" t="inlineStr">
         <is>
-          <t>s23 plus top quality display vivid sharp bright color look natural ✨️ problem watherever fhd qhd 4k 8k pleasure watch movee</t>
+          <t>s23 plus top quality display vivid sharp bright color look natural problem watherever fhd qhd 4k 8k pleasure watch movee</t>
         </is>
       </c>
     </row>
@@ -25034,7 +25034,7 @@
       </c>
       <c r="D1088" t="inlineStr">
         <is>
-          <t>i’m guess 2k resolution know 1440… explains market gimmick work get fact right 1920 2k 2000 pixel range whether like</t>
+          <t>im guess 2k resolution know 1440 explain market gimmick work get fact right 1920 2k 2000 pixel range whether like</t>
         </is>
       </c>
     </row>
@@ -25056,7 +25056,7 @@
       </c>
       <c r="D1089" t="inlineStr">
         <is>
-          <t>learn read 2000 2001 2010 1920 2k literally nobody considers 1920×1080 2k stop</t>
+          <t>learn read 2000 2001 2010 1920 2k literally nobody considers 19201080 2k stop</t>
         </is>
       </c>
     </row>
@@ -25189,7 +25189,7 @@
       </c>
       <c r="D1095" t="inlineStr">
         <is>
-          <t>2k name derive large half pixel measurement 2048 represent 2000 pixel mean display resolution great 2048 × 1080 describe 2k</t>
+          <t>2k name derive large half pixel measurement 2048 represent 2000 pixel mean display resolution great 2048 1080 describe 2k</t>
         </is>
       </c>
     </row>
@@ -25351,7 +25351,7 @@
       </c>
       <c r="D1102" t="inlineStr">
         <is>
-          <t>thanks lot 😊</t>
+          <t>thanks lot</t>
         </is>
       </c>
     </row>
@@ -25794,7 +25794,7 @@
       </c>
       <c r="D1122" t="inlineStr">
         <is>
-          <t>s23 plus top quality display vivid sharp bright color look natural ✨️ problem watherever fhd qhd 4k 8k pleasure watch movee</t>
+          <t>s23 plus top quality display vivid sharp bright color look natural problem watherever fhd qhd 4k 8k pleasure watch movee</t>
         </is>
       </c>
     </row>
@@ -25929,7 +25929,7 @@
       </c>
       <c r="D1128" t="inlineStr">
         <is>
-          <t>i’m guess 2k resolution know 1440… explains market gimmick work get fact right 1920 2k 2000 pixel range whether like</t>
+          <t>im guess 2k resolution know 1440 explain market gimmick work get fact right 1920 2k 2000 pixel range whether like</t>
         </is>
       </c>
     </row>
@@ -25951,7 +25951,7 @@
       </c>
       <c r="D1129" t="inlineStr">
         <is>
-          <t>learn read 2000 2001 2010 1920 2k literally nobody considers 1920×1080 2k stop</t>
+          <t>learn read 2000 2001 2010 1920 2k literally nobody considers 19201080 2k stop</t>
         </is>
       </c>
     </row>
@@ -26084,7 +26084,7 @@
       </c>
       <c r="D1135" t="inlineStr">
         <is>
-          <t>2k name derive large half pixel measurement 2048 represent 2000 pixel mean display resolution great 2048 × 1080 describe 2k</t>
+          <t>2k name derive large half pixel measurement 2048 represent 2000 pixel mean display resolution great 2048 1080 describe 2k</t>
         </is>
       </c>
     </row>
@@ -26246,7 +26246,7 @@
       </c>
       <c r="D1142" t="inlineStr">
         <is>
-          <t>thanks lot 😊</t>
+          <t>thanks lot</t>
         </is>
       </c>
     </row>
@@ -26423,7 +26423,7 @@
       </c>
       <c r="D1150" t="inlineStr">
         <is>
-          <t>1080×1920 2k yall get wrong infos 1080×1920 full hd resolution</t>
+          <t>10801920 2k yall get wrong infos 10801920 full hd resolution</t>
         </is>
       </c>
     </row>
@@ -26445,7 +26445,7 @@
       </c>
       <c r="D1151" t="inlineStr">
         <is>
-          <t>great phone dont look nagitive view use form two month complain great batree full day heavy us nice fhd display 1700 nit size perfect blindly go price reduce one two month satisfy 😌</t>
+          <t>great phone dont look nagitive view use form two month complain great batree full day heavy us nice fhd display 1700 nit size perfect blindly go price reduce one two month satisfy</t>
         </is>
       </c>
     </row>
@@ -26634,7 +26634,7 @@
       </c>
       <c r="D1159" t="inlineStr">
         <is>
-          <t>1920x1080 fhd 2000 pixel qhd 3000 pixel uhd 😂 love people dont know squad try proof thing wrong way</t>
+          <t>1920x1080 fhd 2000 pixel qhd 3000 pixel uhd love people dont know squad try proof thing wrong way</t>
         </is>
       </c>
     </row>
@@ -26836,7 +26836,7 @@
       </c>
       <c r="D1168" t="inlineStr">
         <is>
-          <t>i’m guess 2k resolution know 1440… explains market gimmick work get fact right 1920 2k 2000 pixel range whether like</t>
+          <t>im guess 2k resolution know 1440 explain market gimmick work get fact right 1920 2k 2000 pixel range whether like</t>
         </is>
       </c>
     </row>
@@ -26858,7 +26858,7 @@
       </c>
       <c r="D1169" t="inlineStr">
         <is>
-          <t>learn read 2000 2001 2010 1920 2k literally nobody considers 1920×1080 2k stop</t>
+          <t>learn read 2000 2001 2010 1920 2k literally nobody considers 19201080 2k stop</t>
         </is>
       </c>
     </row>
@@ -26991,7 +26991,7 @@
       </c>
       <c r="D1175" t="inlineStr">
         <is>
-          <t>2k name derive large half pixel measurement 2048 represent 2000 pixel mean display resolution great 2048 × 1080 describe 2k</t>
+          <t>2k name derive large half pixel measurement 2048 represent 2000 pixel mean display resolution great 2048 1080 describe 2k</t>
         </is>
       </c>
     </row>
@@ -27153,7 +27153,7 @@
       </c>
       <c r="D1182" t="inlineStr">
         <is>
-          <t>thanks lot 😊</t>
+          <t>thanks lot</t>
         </is>
       </c>
     </row>
@@ -27330,7 +27330,7 @@
       </c>
       <c r="D1190" t="inlineStr">
         <is>
-          <t>1080×1920 2k yall get wrong infos 1080×1920 full hd resolution</t>
+          <t>10801920 2k yall get wrong infos 10801920 full hd resolution</t>
         </is>
       </c>
     </row>
@@ -27352,7 +27352,7 @@
       </c>
       <c r="D1191" t="inlineStr">
         <is>
-          <t>great phone dont look nagitive view use form two month complain great batree full day heavy us nice fhd display 1700 nit size perfect blindly go price reduce one two month satisfy 😌</t>
+          <t>great phone dont look nagitive view use form two month complain great batree full day heavy us nice fhd display 1700 nit size perfect blindly go price reduce one two month satisfy</t>
         </is>
       </c>
     </row>
@@ -27541,7 +27541,7 @@
       </c>
       <c r="D1199" t="inlineStr">
         <is>
-          <t>1920x1080 fhd 2000 pixel qhd 3000 pixel uhd 😂 love people dont know squad try proof thing wrong way</t>
+          <t>1920x1080 fhd 2000 pixel qhd 3000 pixel uhd love people dont know squad try proof thing wrong way</t>
         </is>
       </c>
     </row>
@@ -27701,7 +27701,7 @@
       </c>
       <c r="D1206" t="inlineStr">
         <is>
-          <t>14 pro s23 excellent sluggish 🥰 even s23 hold background process well 14 pro cough cough io problem 🤪</t>
+          <t>14 pro s23 excellent sluggish even s23 hold background process well 14 pro cough cough io problem</t>
         </is>
       </c>
     </row>
@@ -28244,7 +28244,7 @@
       </c>
       <c r="D1230" t="inlineStr">
         <is>
-          <t>1080×1920 2k yall get wrong infos 1080×1920 full hd resolution</t>
+          <t>10801920 2k yall get wrong infos 10801920 full hd resolution</t>
         </is>
       </c>
     </row>
@@ -28266,7 +28266,7 @@
       </c>
       <c r="D1231" t="inlineStr">
         <is>
-          <t>great phone dont look nagitive view use form two month complain great batree full day heavy us nice fhd display 1700 nit size perfect blindly go price reduce one two month satisfy 😌</t>
+          <t>great phone dont look nagitive view use form two month complain great batree full day heavy us nice fhd display 1700 nit size perfect blindly go price reduce one two month satisfy</t>
         </is>
       </c>
     </row>
@@ -28455,7 +28455,7 @@
       </c>
       <c r="D1239" t="inlineStr">
         <is>
-          <t>1920x1080 fhd 2000 pixel qhd 3000 pixel uhd 😂 love people dont know squad try proof thing wrong way</t>
+          <t>1920x1080 fhd 2000 pixel qhd 3000 pixel uhd love people dont know squad try proof thing wrong way</t>
         </is>
       </c>
     </row>
@@ -28615,7 +28615,7 @@
       </c>
       <c r="D1246" t="inlineStr">
         <is>
-          <t>14 pro s23 excellent sluggish 🥰 even s23 hold background process well 14 pro cough cough io problem 🤪</t>
+          <t>14 pro s23 excellent sluggish even s23 hold background process well 14 pro cough cough io problem</t>
         </is>
       </c>
     </row>
@@ -29025,7 +29025,7 @@
       </c>
       <c r="D1264" t="inlineStr">
         <is>
-          <t>ask £1100 current climate pathetic colour seriously</t>
+          <t>ask 1100 current climate pathetic colour seriously</t>
         </is>
       </c>
     </row>
@@ -29524,7 +29524,7 @@
       </c>
       <c r="D1286" t="inlineStr">
         <is>
-          <t>14 pro s23 excellent sluggish 🥰 even s23 hold background process well 14 pro cough cough io problem 🤪</t>
+          <t>14 pro s23 excellent sluggish even s23 hold background process well 14 pro cough cough io problem</t>
         </is>
       </c>
     </row>
@@ -29934,7 +29934,7 @@
       </c>
       <c r="D1304" t="inlineStr">
         <is>
-          <t>ask £1100 current climate pathetic colour seriously</t>
+          <t>ask 1100 current climate pathetic colour seriously</t>
         </is>
       </c>
     </row>
@@ -30767,7 +30767,7 @@
       </c>
       <c r="D1341" t="inlineStr">
         <is>
-          <t>phone near thousand dollar still uhd option think gimics sell ultra dont like policy 😒</t>
+          <t>phone near thousand dollar still uhd option think gimics sell ultra dont like policy</t>
         </is>
       </c>
     </row>
@@ -30833,7 +30833,7 @@
       </c>
       <c r="D1344" t="inlineStr">
         <is>
-          <t>ask £1100 current climate pathetic colour seriously</t>
+          <t>ask 1100 current climate pathetic colour seriously</t>
         </is>
       </c>
     </row>
@@ -31666,7 +31666,7 @@
       </c>
       <c r="D1381" t="inlineStr">
         <is>
-          <t>phone near thousand dollar still uhd option think gimics sell ultra dont like policy 😒</t>
+          <t>phone near thousand dollar still uhd option think gimics sell ultra dont like policy</t>
         </is>
       </c>
     </row>
@@ -32137,7 +32137,7 @@
       </c>
       <c r="D1402" t="inlineStr">
         <is>
-          <t>25 watt e enough difference full charge 10 minute minor watt charger produce heat batree good batreelife👍</t>
+          <t>25 watt e enough difference full charge 10 minute minor watt charger produce heat batree good batreelife</t>
         </is>
       </c>
     </row>
@@ -32561,7 +32561,7 @@
       </c>
       <c r="D1421" t="inlineStr">
         <is>
-          <t>phone near thousand dollar still uhd option think gimics sell ultra dont like policy 😒</t>
+          <t>phone near thousand dollar still uhd option think gimics sell ultra dont like policy</t>
         </is>
       </c>
     </row>
@@ -33032,7 +33032,7 @@
       </c>
       <c r="D1442" t="inlineStr">
         <is>
-          <t>25 watt e enough difference full charge 10 minute minor watt charger produce heat batree good batreelife👍</t>
+          <t>25 watt e enough difference full charge 10 minute minor watt charger produce heat batree good batreelife</t>
         </is>
       </c>
     </row>
@@ -33924,7 +33924,7 @@
       </c>
       <c r="D1482" t="inlineStr">
         <is>
-          <t>25 watt e enough difference full charge 10 minute minor watt charger produce heat batree good batreelife👍</t>
+          <t>25 watt e enough difference full charge 10 minute minor watt charger produce heat batree good batreelife</t>
         </is>
       </c>
     </row>
@@ -34545,7 +34545,7 @@
       </c>
       <c r="D1510" t="inlineStr">
         <is>
-          <t>perfect balance phone big like ultra small like s23 camera decent nothing matter 200 mp 50 mp output fine happy purchaseno heating display superb sound great batree decrease speed slow even whole night 2 percent perfect 👌</t>
+          <t>perfect balance phone big like ultra small like s23 camera decent nothing matter 200 mp 50 mp output fine happy purchaseno heating display superb sound great batree decrease speed slow even whole night 2 percent perfect</t>
         </is>
       </c>
     </row>
@@ -34812,7 +34812,7 @@
       </c>
       <c r="D1521" t="inlineStr">
         <is>
-          <t>think right rear camera set s20 fe sd beat flagship till front camera well s23 plus switched form fe feeling much change display well shit😪</t>
+          <t>think right rear camera set s20 fe sd beat flagship till front camera well s23 plus switched form fe feeling much change display well shit</t>
         </is>
       </c>
     </row>
@@ -35457,7 +35457,7 @@
       </c>
       <c r="D1550" t="inlineStr">
         <is>
-          <t>perfect balance phone big like ultra small like s23 camera decent nothing matter 200 mp 50 mp output fine happy purchaseno heating display superb sound great batree decrease speed slow even whole night 2 percent perfect 👌</t>
+          <t>perfect balance phone big like ultra small like s23 camera decent nothing matter 200 mp 50 mp output fine happy purchaseno heating display superb sound great batree decrease speed slow even whole night 2 percent perfect</t>
         </is>
       </c>
     </row>
@@ -35724,7 +35724,7 @@
       </c>
       <c r="D1561" t="inlineStr">
         <is>
-          <t>think right rear camera set s20 fe sd beat flagship till front camera well s23 plus switched form fe feeling much change display well shit😪</t>
+          <t>think right rear camera set s20 fe sd beat flagship till front camera well s23 plus switched form fe feeling much change display well shit</t>
         </is>
       </c>
     </row>
@@ -36187,7 +36187,7 @@
       </c>
       <c r="D1581" t="inlineStr">
         <is>
-          <t>yeah really never compare phone’s ppi tvmonitors screen</t>
+          <t>yeah really never compare phone ppi tvmonitors screen</t>
         </is>
       </c>
     </row>
@@ -36387,7 +36387,7 @@
       </c>
       <c r="D1590" t="inlineStr">
         <is>
-          <t>perfect balance phone big like ultra small like s23 camera decent nothing matter 200 mp 50 mp output fine happy purchaseno heating display superb sound great batree decrease speed slow even whole night 2 percent perfect 👌</t>
+          <t>perfect balance phone big like ultra small like s23 camera decent nothing matter 200 mp 50 mp output fine happy purchaseno heating display superb sound great batree decrease speed slow even whole night 2 percent perfect</t>
         </is>
       </c>
     </row>
@@ -36654,7 +36654,7 @@
       </c>
       <c r="D1601" t="inlineStr">
         <is>
-          <t>think right rear camera set s20 fe sd beat flagship till front camera well s23 plus switched form fe feeling much change display well shit😪</t>
+          <t>think right rear camera set s20 fe sd beat flagship till front camera well s23 plus switched form fe feeling much change display well shit</t>
         </is>
       </c>
     </row>
@@ -37117,7 +37117,7 @@
       </c>
       <c r="D1621" t="inlineStr">
         <is>
-          <t>yeah really never compare phone’s ppi tvmonitors screen</t>
+          <t>yeah really never compare phone ppi tvmonitors screen</t>
         </is>
       </c>
     </row>
@@ -37315,7 +37315,7 @@
       </c>
       <c r="D1630" t="inlineStr">
         <is>
-          <t>thinkig purchase s23 plus change mind s23 ppi 425 small screen well go base s23 samsung give qhd plus model would perfect phone plus model happy witn s23 compact size vivd screen crisp diplay nits burn eye well go low nit display heavy user cant use nit display without eyewear longtime👍</t>
+          <t>thinkig purchase s23 plus change mind s23 ppi 425 small screen well go base s23 samsung give qhd plus model would perfect phone plus model happy witn s23 compact size vivd screen crisp diplay nits burn eye well go low nit display heavy user cant use nit display without eyewear longtime</t>
         </is>
       </c>
     </row>
@@ -38032,7 +38032,7 @@
       </c>
       <c r="D1661" t="inlineStr">
         <is>
-          <t>yeah really never compare phone’s ppi tvmonitors screen</t>
+          <t>yeah really never compare phone ppi tvmonitors screen</t>
         </is>
       </c>
     </row>
@@ -38230,7 +38230,7 @@
       </c>
       <c r="D1670" t="inlineStr">
         <is>
-          <t>thinkig purchase s23 plus change mind s23 ppi 425 small screen well go base s23 samsung give qhd plus model would perfect phone plus model happy witn s23 compact size vivd screen crisp diplay nits burn eye well go low nit display heavy user cant use nit display without eyewear longtime👍</t>
+          <t>thinkig purchase s23 plus change mind s23 ppi 425 small screen well go base s23 samsung give qhd plus model would perfect phone plus model happy witn s23 compact size vivd screen crisp diplay nits burn eye well go low nit display heavy user cant use nit display without eyewear longtime</t>
         </is>
       </c>
     </row>
@@ -39133,7 +39133,7 @@
       </c>
       <c r="D1710" t="inlineStr">
         <is>
-          <t>thinkig purchase s23 plus change mind s23 ppi 425 small screen well go base s23 samsung give qhd plus model would perfect phone plus model happy witn s23 compact size vivd screen crisp diplay nits burn eye well go low nit display heavy user cant use nit display without eyewear longtime👍</t>
+          <t>thinkig purchase s23 plus change mind s23 ppi 425 small screen well go base s23 samsung give qhd plus model would perfect phone plus model happy witn s23 compact size vivd screen crisp diplay nits burn eye well go low nit display heavy user cant use nit display without eyewear longtime</t>
         </is>
       </c>
     </row>
@@ -42988,7 +42988,7 @@
       </c>
       <c r="D1881" t="inlineStr">
         <is>
-          <t>13 pro like mid range it’s class 14 pro</t>
+          <t>13 pro like mid range class 14 pro</t>
         </is>
       </c>
     </row>
@@ -43892,7 +43892,7 @@
       </c>
       <c r="D1921" t="inlineStr">
         <is>
-          <t>13 pro like mid range it’s class 14 pro</t>
+          <t>13 pro like mid range class 14 pro</t>
         </is>
       </c>
     </row>
@@ -44147,7 +44147,7 @@
       </c>
       <c r="D1932" t="inlineStr">
         <is>
-          <t>go buy bugmi 🐛 one care comment necessary</t>
+          <t>go buy bugmi one care comment necessary</t>
         </is>
       </c>
     </row>
@@ -44236,7 +44236,7 @@
       </c>
       <c r="D1936" t="inlineStr">
         <is>
-          <t>there’sa downgrade camera telephoto ois</t>
+          <t>theresa downgrade camera telephoto ois</t>
         </is>
       </c>
     </row>
@@ -44803,7 +44803,7 @@
       </c>
       <c r="D1961" t="inlineStr">
         <is>
-          <t>13 pro like mid range it’s class 14 pro</t>
+          <t>13 pro like mid range class 14 pro</t>
         </is>
       </c>
     </row>
@@ -45058,7 +45058,7 @@
       </c>
       <c r="D1972" t="inlineStr">
         <is>
-          <t>go buy bugmi 🐛 one care comment necessary</t>
+          <t>go buy bugmi one care comment necessary</t>
         </is>
       </c>
     </row>
@@ -45147,7 +45147,7 @@
       </c>
       <c r="D1976" t="inlineStr">
         <is>
-          <t>there’sa downgrade camera telephoto ois</t>
+          <t>theresa downgrade camera telephoto ois</t>
         </is>
       </c>
     </row>
@@ -45953,7 +45953,7 @@
       </c>
       <c r="D2012" t="inlineStr">
         <is>
-          <t>go buy bugmi 🐛 one care comment necessary</t>
+          <t>go buy bugmi one care comment necessary</t>
         </is>
       </c>
     </row>
@@ -46042,7 +46042,7 @@
       </c>
       <c r="D2016" t="inlineStr">
         <is>
-          <t>there’sa downgrade camera telephoto ois</t>
+          <t>theresa downgrade camera telephoto ois</t>
         </is>
       </c>
     </row>
@@ -46712,7 +46712,7 @@
       </c>
       <c r="D2046" t="inlineStr">
         <is>
-          <t>it’s ip68</t>
+          <t>ip68</t>
         </is>
       </c>
     </row>
@@ -46734,7 +46734,7 @@
       </c>
       <c r="D2047" t="inlineStr">
         <is>
-          <t>don’t still could see big difference</t>
+          <t>dont still could see big difference</t>
         </is>
       </c>
     </row>
@@ -46898,7 +46898,7 @@
       </c>
       <c r="D2054" t="inlineStr">
         <is>
-          <t>i’m techie 8gb ram enough damn 1080p</t>
+          <t>im techie 8gb ram enough damn 1080p</t>
         </is>
       </c>
     </row>
@@ -47054,7 +47054,7 @@
       </c>
       <c r="D2061" t="inlineStr">
         <is>
-          <t>perfectly can’t even see 17x difference xd</t>
+          <t>perfectly cant even see 17x difference xd</t>
         </is>
       </c>
     </row>
@@ -47076,7 +47076,7 @@
       </c>
       <c r="D2062" t="inlineStr">
         <is>
-          <t>first buy midrange phone want 1080p qhd second even buy highend phone still use 1080p unless it’s iphone far know might wrong</t>
+          <t>first buy midrange phone want 1080p qhd second even buy highend phone still use 1080p unless iphone far know might wrong</t>
         </is>
       </c>
     </row>
@@ -47098,7 +47098,7 @@
       </c>
       <c r="D2063" t="inlineStr">
         <is>
-          <t>yeah there’s justification big screen provider make “flagship” i’m sure heshe would justification apple samsung even make 7’ phone 100100 pixel xd</t>
+          <t>yeah there justification big screen provider make flagship im sure heshe would justification apple samsung even make 7 phone 100100 pixel xd</t>
         </is>
       </c>
     </row>
@@ -47612,7 +47612,7 @@
       </c>
       <c r="D2086" t="inlineStr">
         <is>
-          <t>it’s ip68</t>
+          <t>ip68</t>
         </is>
       </c>
     </row>
@@ -47634,7 +47634,7 @@
       </c>
       <c r="D2087" t="inlineStr">
         <is>
-          <t>don’t still could see big difference</t>
+          <t>dont still could see big difference</t>
         </is>
       </c>
     </row>
@@ -47798,7 +47798,7 @@
       </c>
       <c r="D2094" t="inlineStr">
         <is>
-          <t>i’m techie 8gb ram enough damn 1080p</t>
+          <t>im techie 8gb ram enough damn 1080p</t>
         </is>
       </c>
     </row>
@@ -47954,7 +47954,7 @@
       </c>
       <c r="D2101" t="inlineStr">
         <is>
-          <t>perfectly can’t even see 17x difference xd</t>
+          <t>perfectly cant even see 17x difference xd</t>
         </is>
       </c>
     </row>
@@ -47976,7 +47976,7 @@
       </c>
       <c r="D2102" t="inlineStr">
         <is>
-          <t>first buy midrange phone want 1080p qhd second even buy highend phone still use 1080p unless it’s iphone far know might wrong</t>
+          <t>first buy midrange phone want 1080p qhd second even buy highend phone still use 1080p unless iphone far know might wrong</t>
         </is>
       </c>
     </row>
@@ -47998,7 +47998,7 @@
       </c>
       <c r="D2103" t="inlineStr">
         <is>
-          <t>yeah there’s justification big screen provider make “flagship” i’m sure heshe would justification apple samsung even make 7’ phone 100100 pixel xd</t>
+          <t>yeah there justification big screen provider make flagship im sure heshe would justification apple samsung even make 7 phone 100100 pixel xd</t>
         </is>
       </c>
     </row>
@@ -48020,7 +48020,7 @@
       </c>
       <c r="D2104" t="inlineStr">
         <is>
-          <t>i’m currently use iphone se2 reno5 4g s7 edge past broke s7 edge buy new phone i’ve notice clear difference fhd qhd unlike great eyesight it’s fault can’t see difference xd</t>
+          <t>im currently use iphone se2 reno5 4g s7 edge past broke s7 edge buy new phone ive notice clear difference fhd qhd unlike great eyesight fault cant see difference xd</t>
         </is>
       </c>
     </row>
@@ -48209,7 +48209,7 @@
       </c>
       <c r="D2112" t="inlineStr">
         <is>
-          <t>i’ve use 1080p monitor they’re blurry hell</t>
+          <t>ive use 1080p monitor theyre blurry hell</t>
         </is>
       </c>
     </row>
@@ -48231,7 +48231,7 @@
       </c>
       <c r="D2113" t="inlineStr">
         <is>
-          <t>vanilla xiaomi 11 qhd screen didn’t know</t>
+          <t>vanilla xiaomi 11 qhd screen didnt know</t>
         </is>
       </c>
     </row>
@@ -48275,7 +48275,7 @@
       </c>
       <c r="D2115" t="inlineStr">
         <is>
-          <t>it’s problem bad eyesight</t>
+          <t>problem bad eyesight</t>
         </is>
       </c>
     </row>
@@ -48297,7 +48297,7 @@
       </c>
       <c r="D2116" t="inlineStr">
         <is>
-          <t>need go ophthalmologist phone qhd fhd screen i’ve see clear difference</t>
+          <t>need go ophthalmologist phone qhd fhd screen ive see clear difference</t>
         </is>
       </c>
     </row>
@@ -48386,7 +48386,7 @@
       </c>
       <c r="D2120" t="inlineStr">
         <is>
-          <t>problem money save 😉</t>
+          <t>problem money save</t>
         </is>
       </c>
     </row>
@@ -48526,7 +48526,7 @@
       </c>
       <c r="D2126" t="inlineStr">
         <is>
-          <t>it’s ip68</t>
+          <t>ip68</t>
         </is>
       </c>
     </row>
@@ -48548,7 +48548,7 @@
       </c>
       <c r="D2127" t="inlineStr">
         <is>
-          <t>don’t still could see big difference</t>
+          <t>dont still could see big difference</t>
         </is>
       </c>
     </row>
@@ -48712,7 +48712,7 @@
       </c>
       <c r="D2134" t="inlineStr">
         <is>
-          <t>i’m techie 8gb ram enough damn 1080p</t>
+          <t>im techie 8gb ram enough damn 1080p</t>
         </is>
       </c>
     </row>
@@ -48868,7 +48868,7 @@
       </c>
       <c r="D2141" t="inlineStr">
         <is>
-          <t>perfectly can’t even see 17x difference xd</t>
+          <t>perfectly cant even see 17x difference xd</t>
         </is>
       </c>
     </row>
@@ -48890,7 +48890,7 @@
       </c>
       <c r="D2142" t="inlineStr">
         <is>
-          <t>first buy midrange phone want 1080p qhd second even buy highend phone still use 1080p unless it’s iphone far know might wrong</t>
+          <t>first buy midrange phone want 1080p qhd second even buy highend phone still use 1080p unless iphone far know might wrong</t>
         </is>
       </c>
     </row>
@@ -48912,7 +48912,7 @@
       </c>
       <c r="D2143" t="inlineStr">
         <is>
-          <t>yeah there’s justification big screen provider make “flagship” i’m sure heshe would justification apple samsung even make 7’ phone 100100 pixel xd</t>
+          <t>yeah there justification big screen provider make flagship im sure heshe would justification apple samsung even make 7 phone 100100 pixel xd</t>
         </is>
       </c>
     </row>
@@ -48934,7 +48934,7 @@
       </c>
       <c r="D2144" t="inlineStr">
         <is>
-          <t>i’m currently use iphone se2 reno5 4g s7 edge past broke s7 edge buy new phone i’ve notice clear difference fhd qhd unlike great eyesight it’s fault can’t see difference xd</t>
+          <t>im currently use iphone se2 reno5 4g s7 edge past broke s7 edge buy new phone ive notice clear difference fhd qhd unlike great eyesight fault cant see difference xd</t>
         </is>
       </c>
     </row>
@@ -49123,7 +49123,7 @@
       </c>
       <c r="D2152" t="inlineStr">
         <is>
-          <t>i’ve use 1080p monitor they’re blurry hell</t>
+          <t>ive use 1080p monitor theyre blurry hell</t>
         </is>
       </c>
     </row>
@@ -49145,7 +49145,7 @@
       </c>
       <c r="D2153" t="inlineStr">
         <is>
-          <t>vanilla xiaomi 11 qhd screen didn’t know</t>
+          <t>vanilla xiaomi 11 qhd screen didnt know</t>
         </is>
       </c>
     </row>
@@ -49189,7 +49189,7 @@
       </c>
       <c r="D2155" t="inlineStr">
         <is>
-          <t>it’s problem bad eyesight</t>
+          <t>problem bad eyesight</t>
         </is>
       </c>
     </row>
@@ -49211,7 +49211,7 @@
       </c>
       <c r="D2156" t="inlineStr">
         <is>
-          <t>need go ophthalmologist phone qhd fhd screen i’ve see clear difference</t>
+          <t>need go ophthalmologist phone qhd fhd screen ive see clear difference</t>
         </is>
       </c>
     </row>
@@ -49300,7 +49300,7 @@
       </c>
       <c r="D2160" t="inlineStr">
         <is>
-          <t>problem money save 😉</t>
+          <t>problem money save</t>
         </is>
       </c>
     </row>
@@ -49458,7 +49458,7 @@
       </c>
       <c r="D2167" t="inlineStr">
         <is>
-          <t>course wqhd well fhd like duuuhhh 💡 youve never use youtube 1440 mode youre internet expensive Rolling On The Floor Laughing theres clearly difference need appointment eye doctor something youre defend bad practice greedy company use midrange display highend flagship cost 1000 euro sure youre trolley troll 🤣</t>
+          <t>course wqhd well fhd like duuuhhh youve never use youtube 1440 mode youre internet expensive Rolling On The Floor Laughing theres clearly difference need appointment eye doctor something youre defend bad practice greedy company use midrange display highend flagship cost 1000 euro sure youre trolley troll</t>
         </is>
       </c>
     </row>
@@ -49542,7 +49542,7 @@
       </c>
       <c r="D2171" t="inlineStr">
         <is>
-          <t>imagine compare 2 year old phone late phone 🤣</t>
+          <t>imagine compare 2 year old phone late phone</t>
         </is>
       </c>
     </row>
@@ -49710,7 +49710,7 @@
       </c>
       <c r="D2178" t="inlineStr">
         <is>
-          <t>past think samsung best phone company worldbut feel possible always think customer money value2021 2023 feature developedwhy thisapple company think customersbut samsung count ex ip68 water dust resistance15 meter 30mins apple 6m 30mins apple selfi camera best different toolsbut samsung least give 5year software hardware warranty best camera video record capability 4k24253060fps 1080p253060120240fps 10bit hdr dolby vision hdr 60fps prores cinematic mode 4k2430fps stereo sound rec selfie camera single 12 mp f19 23mm wide 136 pdaf ois unconfirmed sl 3d depthbiometrics sensor feature hdr cinematic mode 4k2430fps video 4k24253060fps 1080p253060120fps gyroeis please samsung think usthen best phone company world even apple🍁😭😭😭😭😭</t>
+          <t>past think samsung best phone company worldbut feel possible always think customer money value2021 2023 feature developedwhy thisapple company think customersbut samsung count ex ip68 water dust resistance15 meter 30mins apple 6m 30mins apple selfi camera best different toolsbut samsung least give 5year software hardware warranty best camera video record capability 4k24253060fps 1080p253060120240fps 10bit hdr dolby vision hdr 60fps prores cinematic mode 4k2430fps stereo sound rec selfie camera single 12 mp f19 23mm wide 136 pdaf ois unconfirmed sl 3d depthbiometrics sensor feature hdr cinematic mode 4k2430fps video 4k24253060fps 1080p253060120fps gyroeis please samsung think usthen best phone company world even apple</t>
         </is>
       </c>
     </row>
@@ -49843,7 +49843,7 @@
       </c>
       <c r="D2184" t="inlineStr">
         <is>
-          <t>i’m currently use iphone se2 reno5 4g s7 edge past broke s7 edge buy new phone i’ve notice clear difference fhd qhd unlike great eyesight it’s fault can’t see difference xd</t>
+          <t>im currently use iphone se2 reno5 4g s7 edge past broke s7 edge buy new phone ive notice clear difference fhd qhd unlike great eyesight fault cant see difference xd</t>
         </is>
       </c>
     </row>
@@ -50032,7 +50032,7 @@
       </c>
       <c r="D2192" t="inlineStr">
         <is>
-          <t>i’ve use 1080p monitor they’re blurry hell</t>
+          <t>ive use 1080p monitor theyre blurry hell</t>
         </is>
       </c>
     </row>
@@ -50054,7 +50054,7 @@
       </c>
       <c r="D2193" t="inlineStr">
         <is>
-          <t>vanilla xiaomi 11 qhd screen didn’t know</t>
+          <t>vanilla xiaomi 11 qhd screen didnt know</t>
         </is>
       </c>
     </row>
@@ -50098,7 +50098,7 @@
       </c>
       <c r="D2195" t="inlineStr">
         <is>
-          <t>it’s problem bad eyesight</t>
+          <t>problem bad eyesight</t>
         </is>
       </c>
     </row>
@@ -50120,7 +50120,7 @@
       </c>
       <c r="D2196" t="inlineStr">
         <is>
-          <t>need go ophthalmologist phone qhd fhd screen i’ve see clear difference</t>
+          <t>need go ophthalmologist phone qhd fhd screen ive see clear difference</t>
         </is>
       </c>
     </row>
@@ -50209,7 +50209,7 @@
       </c>
       <c r="D2200" t="inlineStr">
         <is>
-          <t>problem money save 😉</t>
+          <t>problem money save</t>
         </is>
       </c>
     </row>
@@ -50367,7 +50367,7 @@
       </c>
       <c r="D2207" t="inlineStr">
         <is>
-          <t>course wqhd well fhd like duuuhhh 💡 youve never use youtube 1440 mode youre internet expensive Rolling On The Floor Laughing theres clearly difference need appointment eye doctor something youre defend bad practice greedy company use midrange display highend flagship cost 1000 euro sure youre trolley troll 🤣</t>
+          <t>course wqhd well fhd like duuuhhh youve never use youtube 1440 mode youre internet expensive Rolling On The Floor Laughing theres clearly difference need appointment eye doctor something youre defend bad practice greedy company use midrange display highend flagship cost 1000 euro sure youre trolley troll</t>
         </is>
       </c>
     </row>
@@ -50451,7 +50451,7 @@
       </c>
       <c r="D2211" t="inlineStr">
         <is>
-          <t>imagine compare 2 year old phone late phone 🤣</t>
+          <t>imagine compare 2 year old phone late phone</t>
         </is>
       </c>
     </row>
@@ -50619,7 +50619,7 @@
       </c>
       <c r="D2218" t="inlineStr">
         <is>
-          <t>past think samsung best phone company worldbut feel possible always think customer money value2021 2023 feature developedwhy thisapple company think customersbut samsung count ex ip68 water dust resistance15 meter 30mins apple 6m 30mins apple selfi camera best different toolsbut samsung least give 5year software hardware warranty best camera video record capability 4k24253060fps 1080p253060120240fps 10bit hdr dolby vision hdr 60fps prores cinematic mode 4k2430fps stereo sound rec selfie camera single 12 mp f19 23mm wide 136 pdaf ois unconfirmed sl 3d depthbiometrics sensor feature hdr cinematic mode 4k2430fps video 4k24253060fps 1080p253060120fps gyroeis please samsung think usthen best phone company world even apple🍁😭😭😭😭😭</t>
+          <t>past think samsung best phone company worldbut feel possible always think customer money value2021 2023 feature developedwhy thisapple company think customersbut samsung count ex ip68 water dust resistance15 meter 30mins apple 6m 30mins apple selfi camera best different toolsbut samsung least give 5year software hardware warranty best camera video record capability 4k24253060fps 1080p253060120240fps 10bit hdr dolby vision hdr 60fps prores cinematic mode 4k2430fps stereo sound rec selfie camera single 12 mp f19 23mm wide 136 pdaf ois unconfirmed sl 3d depthbiometrics sensor feature hdr cinematic mode 4k2430fps video 4k24253060fps 1080p253060120fps gyroeis please samsung think usthen best phone company world even apple</t>
         </is>
       </c>
     </row>
@@ -50907,7 +50907,7 @@
       </c>
       <c r="D2231" t="inlineStr">
         <is>
-          <t>dont purchase phone samsung worker fee family please 🙏</t>
+          <t>dont purchase phone samsung worker fee family please</t>
         </is>
       </c>
     </row>
@@ -50997,7 +50997,7 @@
       </c>
       <c r="D2235" t="inlineStr">
         <is>
-          <t>please point get swappable microssd smartphones point slot s23 ultra s23 plus im waiting 🎤💧</t>
+          <t>please point get swappable microssd smartphones point slot s23 ultra s23 plus im waiting</t>
         </is>
       </c>
     </row>
@@ -51050,7 +51050,7 @@
       </c>
       <c r="D2237" t="inlineStr">
         <is>
-          <t>i’m also samsung fan stop justify almost every samsung move p don’t miss microsd</t>
+          <t>im also samsung fan stop justify almost every samsung move p dont miss microsd</t>
         </is>
       </c>
     </row>
@@ -51072,7 +51072,7 @@
       </c>
       <c r="D2238" t="inlineStr">
         <is>
-          <t>they’re make plastic</t>
+          <t>theyre make plastic</t>
         </is>
       </c>
     </row>
@@ -51094,7 +51094,7 @@
       </c>
       <c r="D2239" t="inlineStr">
         <is>
-          <t>disagree screen resolution phone 10802400 screen it’s way bad 1440p it’s normal get midrange phone flagship 8gb ram</t>
+          <t>disagree screen resolution phone 10802400 screen way bad 1440p normal get midrange phone flagship 8gb ram</t>
         </is>
       </c>
     </row>
@@ -51283,7 +51283,7 @@
       </c>
       <c r="D2247" t="inlineStr">
         <is>
-          <t>course wqhd well fhd like duuuhhh 💡 youve never use youtube 1440 mode youre internet expensive Rolling On The Floor Laughing theres clearly difference need appointment eye doctor something youre defend bad practice greedy company use midrange display highend flagship cost 1000 euro sure youre trolley troll 🤣</t>
+          <t>course wqhd well fhd like duuuhhh youve never use youtube 1440 mode youre internet expensive Rolling On The Floor Laughing theres clearly difference need appointment eye doctor something youre defend bad practice greedy company use midrange display highend flagship cost 1000 euro sure youre trolley troll</t>
         </is>
       </c>
     </row>
@@ -51367,7 +51367,7 @@
       </c>
       <c r="D2251" t="inlineStr">
         <is>
-          <t>imagine compare 2 year old phone late phone 🤣</t>
+          <t>imagine compare 2 year old phone late phone</t>
         </is>
       </c>
     </row>
@@ -51535,7 +51535,7 @@
       </c>
       <c r="D2258" t="inlineStr">
         <is>
-          <t>past think samsung best phone company worldbut feel possible always think customer money value2021 2023 feature developedwhy thisapple company think customersbut samsung count ex ip68 water dust resistance15 meter 30mins apple 6m 30mins apple selfi camera best different toolsbut samsung least give 5year software hardware warranty best camera video record capability 4k24253060fps 1080p253060120240fps 10bit hdr dolby vision hdr 60fps prores cinematic mode 4k2430fps stereo sound rec selfie camera single 12 mp f19 23mm wide 136 pdaf ois unconfirmed sl 3d depthbiometrics sensor feature hdr cinematic mode 4k2430fps video 4k24253060fps 1080p253060120fps gyroeis please samsung think usthen best phone company world even apple🍁😭😭😭😭😭</t>
+          <t>past think samsung best phone company worldbut feel possible always think customer money value2021 2023 feature developedwhy thisapple company think customersbut samsung count ex ip68 water dust resistance15 meter 30mins apple 6m 30mins apple selfi camera best different toolsbut samsung least give 5year software hardware warranty best camera video record capability 4k24253060fps 1080p253060120240fps 10bit hdr dolby vision hdr 60fps prores cinematic mode 4k2430fps stereo sound rec selfie camera single 12 mp f19 23mm wide 136 pdaf ois unconfirmed sl 3d depthbiometrics sensor feature hdr cinematic mode 4k2430fps video 4k24253060fps 1080p253060120fps gyroeis please samsung think usthen best phone company world even apple</t>
         </is>
       </c>
     </row>
@@ -51823,7 +51823,7 @@
       </c>
       <c r="D2271" t="inlineStr">
         <is>
-          <t>dont purchase phone samsung worker fee family please 🙏</t>
+          <t>dont purchase phone samsung worker fee family please</t>
         </is>
       </c>
     </row>
@@ -51913,7 +51913,7 @@
       </c>
       <c r="D2275" t="inlineStr">
         <is>
-          <t>please point get swappable microssd smartphones point slot s23 ultra s23 plus im waiting 🎤💧</t>
+          <t>please point get swappable microssd smartphones point slot s23 ultra s23 plus im waiting</t>
         </is>
       </c>
     </row>
@@ -51966,7 +51966,7 @@
       </c>
       <c r="D2277" t="inlineStr">
         <is>
-          <t>i’m also samsung fan stop justify almost every samsung move p don’t miss microsd</t>
+          <t>im also samsung fan stop justify almost every samsung move p dont miss microsd</t>
         </is>
       </c>
     </row>
@@ -51988,7 +51988,7 @@
       </c>
       <c r="D2278" t="inlineStr">
         <is>
-          <t>they’re make plastic</t>
+          <t>theyre make plastic</t>
         </is>
       </c>
     </row>
@@ -52010,7 +52010,7 @@
       </c>
       <c r="D2279" t="inlineStr">
         <is>
-          <t>disagree screen resolution phone 10802400 screen it’s way bad 1440p it’s normal get midrange phone flagship 8gb ram</t>
+          <t>disagree screen resolution phone 10802400 screen way bad 1440p normal get midrange phone flagship 8gb ram</t>
         </is>
       </c>
     </row>
@@ -52221,7 +52221,7 @@
       </c>
       <c r="D2288" t="inlineStr">
         <is>
-          <t>seem like reasonable person mention screen resolution mention obsolete sd card i’m strongly doubt xd p i’m fan cloud storage</t>
+          <t>seem like reasonable person mention screen resolution mention obsolete sd card im strongly doubt xd p im fan cloud storage</t>
         </is>
       </c>
     </row>
@@ -52367,7 +52367,7 @@
       </c>
       <c r="D2294" t="inlineStr">
         <is>
-          <t>1220 eur 💀</t>
+          <t>1220 eur</t>
         </is>
       </c>
     </row>
@@ -52576,7 +52576,7 @@
       </c>
       <c r="D2303" t="inlineStr">
         <is>
-          <t>rip battery health motorola 💀💀</t>
+          <t>rip battery health motorola</t>
         </is>
       </c>
     </row>
@@ -52753,7 +52753,7 @@
       </c>
       <c r="D2311" t="inlineStr">
         <is>
-          <t>dont purchase phone samsung worker fee family please 🙏</t>
+          <t>dont purchase phone samsung worker fee family please</t>
         </is>
       </c>
     </row>
@@ -52843,7 +52843,7 @@
       </c>
       <c r="D2315" t="inlineStr">
         <is>
-          <t>please point get swappable microssd smartphones point slot s23 ultra s23 plus im waiting 🎤💧</t>
+          <t>please point get swappable microssd smartphones point slot s23 ultra s23 plus im waiting</t>
         </is>
       </c>
     </row>
@@ -52896,7 +52896,7 @@
       </c>
       <c r="D2317" t="inlineStr">
         <is>
-          <t>i’m also samsung fan stop justify almost every samsung move p don’t miss microsd</t>
+          <t>im also samsung fan stop justify almost every samsung move p dont miss microsd</t>
         </is>
       </c>
     </row>
@@ -52918,7 +52918,7 @@
       </c>
       <c r="D2318" t="inlineStr">
         <is>
-          <t>they’re make plastic</t>
+          <t>theyre make plastic</t>
         </is>
       </c>
     </row>
@@ -52940,7 +52940,7 @@
       </c>
       <c r="D2319" t="inlineStr">
         <is>
-          <t>disagree screen resolution phone 10802400 screen it’s way bad 1440p it’s normal get midrange phone flagship 8gb ram</t>
+          <t>disagree screen resolution phone 10802400 screen way bad 1440p normal get midrange phone flagship 8gb ram</t>
         </is>
       </c>
     </row>
@@ -53151,7 +53151,7 @@
       </c>
       <c r="D2328" t="inlineStr">
         <is>
-          <t>seem like reasonable person mention screen resolution mention obsolete sd card i’m strongly doubt xd p i’m fan cloud storage</t>
+          <t>seem like reasonable person mention screen resolution mention obsolete sd card im strongly doubt xd p im fan cloud storage</t>
         </is>
       </c>
     </row>
@@ -53297,7 +53297,7 @@
       </c>
       <c r="D2334" t="inlineStr">
         <is>
-          <t>1220 eur 💀</t>
+          <t>1220 eur</t>
         </is>
       </c>
     </row>
@@ -53506,7 +53506,7 @@
       </c>
       <c r="D2343" t="inlineStr">
         <is>
-          <t>rip battery health motorola 💀💀</t>
+          <t>rip battery health motorola</t>
         </is>
       </c>
     </row>
@@ -53748,7 +53748,7 @@
       </c>
       <c r="D2354" t="inlineStr">
         <is>
-          <t>except s23 series use overclocked sd 8 g2 make samsung foundry Laugh My A.. Off</t>
+          <t>except s23 series use overclocked sd 8 g2 make samsung foundry Laugh My A Off</t>
         </is>
       </c>
     </row>
@@ -54064,7 +54064,7 @@
       </c>
       <c r="D2368" t="inlineStr">
         <is>
-          <t>seem like reasonable person mention screen resolution mention obsolete sd card i’m strongly doubt xd p i’m fan cloud storage</t>
+          <t>seem like reasonable person mention screen resolution mention obsolete sd card im strongly doubt xd p im fan cloud storage</t>
         </is>
       </c>
     </row>
@@ -54210,7 +54210,7 @@
       </c>
       <c r="D2374" t="inlineStr">
         <is>
-          <t>1220 eur 💀</t>
+          <t>1220 eur</t>
         </is>
       </c>
     </row>
@@ -54419,7 +54419,7 @@
       </c>
       <c r="D2383" t="inlineStr">
         <is>
-          <t>rip battery health motorola 💀💀</t>
+          <t>rip battery health motorola</t>
         </is>
       </c>
     </row>
@@ -54661,7 +54661,7 @@
       </c>
       <c r="D2394" t="inlineStr">
         <is>
-          <t>except s23 series use overclocked sd 8 g2 make samsung foundry Laugh My A.. Off</t>
+          <t>except s23 series use overclocked sd 8 g2 make samsung foundry Laugh My A Off</t>
         </is>
       </c>
     </row>
@@ -54907,7 +54907,7 @@
       </c>
       <c r="D2405" t="inlineStr">
         <is>
-          <t>samsung 0 bug 😂</t>
+          <t>samsung 0 bug</t>
         </is>
       </c>
     </row>
@@ -55126,7 +55126,7 @@
       </c>
       <c r="D2414" t="inlineStr">
         <is>
-          <t>unofficial price phonandroid base model s23 900€ s23 1200€ s23u 1500€ samsung thank</t>
+          <t>unofficial price phonandroid base model s23 900 s23 1200 s23u 1500 samsung thank</t>
         </is>
       </c>
     </row>

</xml_diff>